<commit_message>
Updated paramter ranges and models to incoroporate updates from Andres, JM, and Carlos. Integrated PMR hydrology into python framework.
</commit_message>
<xml_diff>
--- a/shared_data/Incertidumbre Produccion Industrial.xlsx
+++ b/shared_data/Incertidumbre Produccion Industrial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/FY20/SWCHE102-1000/git/MultiSector_LTS_Chile/shared_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8CAD2DD-B47A-764A-BE79-606E2A89DA69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA6B13A-9B99-094A-9E2E-39396CBA5E11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="460" windowWidth="25680" windowHeight="12900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17760" yWindow="8100" windowWidth="25680" windowHeight="12900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2129,8 +2129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C60BBD-D70C-B745-ABDA-A953F2ECFFF4}">
   <dimension ref="A1:AR28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X3" workbookViewId="0">
-      <selection activeCell="AI14" sqref="AI14"/>
+    <sheetView tabSelected="1" topLeftCell="AI16" workbookViewId="0">
+      <selection activeCell="AI19" sqref="AI19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>